<commit_message>
📝 Added Tabled.pdf file and update previous exercise
WIP
</commit_message>
<xml_diff>
--- a/Week 1/Exercises/Practica01_Layout_Archivo_Secuencial_VictorManuelLavalleCanton.xlsx
+++ b/Week 1/Exercises/Practica01_Layout_Archivo_Secuencial_VictorManuelLavalleCanton.xlsx
@@ -408,7 +408,7 @@
     <t xml:space="preserve">05 VCSAT-CD-POSTAL-F          PIC  9(005).    </t>
   </si>
   <si>
-    <t xml:space="preserve">    0</t>
+    <t>00000 (Error en el archivo, ya que solo hay un 0)</t>
   </si>
   <si>
     <t xml:space="preserve">05 VCSAT-NB-POBLACION-F       PIC  X(030).    </t>
@@ -482,7 +482,7 @@
       <name val="Courier New"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,6 +495,12 @@
         <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -502,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -528,6 +534,10 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf quotePrefix="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf quotePrefix="1" borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -747,7 +757,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="7" width="11.57"/>
-    <col customWidth="1" min="8" max="8" width="68.29"/>
+    <col customWidth="1" min="8" max="8" width="80.14"/>
     <col customWidth="1" min="9" max="26" width="10.71"/>
   </cols>
   <sheetData>
@@ -3470,16 +3480,16 @@
       <c r="Z85" s="2"/>
     </row>
     <row r="86" ht="18.0" customHeight="1">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="7" t="s">
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="12" t="s">
         <v>130</v>
       </c>
       <c r="I86" s="2"/>

</xml_diff>